<commit_message>
Added: New local railway dataset
</commit_message>
<xml_diff>
--- a/datasets/railway/local-railway-RTI/local-injured-deaths.xlsx
+++ b/datasets/railway/local-railway-RTI/local-injured-deaths.xlsx
@@ -2,16 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="1660" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="7760" yWindow="0" windowWidth="21040" windowHeight="17560" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2009" sheetId="1" r:id="rId1"/>
     <sheet name="2010" sheetId="2" r:id="rId2"/>
     <sheet name="2011" sheetId="3" r:id="rId3"/>
     <sheet name="Consolidated" sheetId="4" r:id="rId4"/>
+    <sheet name="Stations" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Stations!$A$1:$C$29</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="152">
   <si>
     <t>Station</t>
   </si>
@@ -382,6 +386,102 @@
   </si>
   <si>
     <t>Aug (D) (2011)</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Andheri</t>
+  </si>
+  <si>
+    <t>Bandra</t>
+  </si>
+  <si>
+    <t>Mumbai Central</t>
+  </si>
+  <si>
+    <t>Boisar</t>
+  </si>
+  <si>
+    <t>Borivali</t>
+  </si>
+  <si>
+    <t>Bhayandar</t>
+  </si>
+  <si>
+    <t>Churchgate</t>
+  </si>
+  <si>
+    <t>Charni Road</t>
+  </si>
+  <si>
+    <t>Dadar</t>
+  </si>
+  <si>
+    <t>Dahisar</t>
+  </si>
+  <si>
+    <t>Elphinstone Road</t>
+  </si>
+  <si>
+    <t>Goregaon</t>
+  </si>
+  <si>
+    <t>Grant Road</t>
+  </si>
+  <si>
+    <t>Jogeshwari</t>
+  </si>
+  <si>
+    <t>Khar Road</t>
+  </si>
+  <si>
+    <t>Kandivli</t>
+  </si>
+  <si>
+    <t>Malad</t>
+  </si>
+  <si>
+    <t>Marine Lines</t>
+  </si>
+  <si>
+    <t>Mira Road</t>
+  </si>
+  <si>
+    <t>Mahim Junction</t>
+  </si>
+  <si>
+    <t>Matunga Road</t>
+  </si>
+  <si>
+    <t>Mahalakshmi</t>
+  </si>
+  <si>
+    <t>Naigaon</t>
+  </si>
+  <si>
+    <t>Nalasopara</t>
+  </si>
+  <si>
+    <t>Lower Parel</t>
+  </si>
+  <si>
+    <t>Santa Cruz</t>
+  </si>
+  <si>
+    <t>Vile Parle</t>
+  </si>
+  <si>
+    <t>Virar</t>
+  </si>
+  <si>
+    <t>Detailed Address</t>
   </si>
 </sst>
 </file>
@@ -444,7 +544,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -486,14 +586,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="44">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -514,6 +618,8 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -534,6 +640,7 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -863,6 +970,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3490,6 +3598,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6117,6 +6226,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8070,10 +8180,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:BO30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14349,4 +14460,463 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="34.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE(C2," station, Mumbai, India")</f>
+        <v>Churchgate station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D29" si="0">CONCATENATE(C3," station, Mumbai, India")</f>
+        <v>Marine Lines station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>Charni Road station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>Grant Road station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>Mumbai Central station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>Mahalakshmi station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower Parel station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>Elphinstone Road station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>Dadar station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>Matunga Road station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>Mahim Junction station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>Bandra station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>Khar Road station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>Santa Cruz station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>Vile Parle station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>Andheri station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>Jogeshwari station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>Goregaon station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>Malad station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>Kandivli station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>Borivali station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>132</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>Dahisar station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>Mira Road station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>Bhayandar station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>Naigaon station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>Boisar station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>Nalasopara station, Mumbai, India</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>Virar station, Mumbai, India</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>